<commit_message>
improve recall by adjusting class weights
</commit_message>
<xml_diff>
--- a/Performance.xlsx
+++ b/Performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/menghan/Documents/PaperIdeas/Yining/water_transfer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50037C84-563F-FB43-960B-94F55E52B713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD54C895-61CA-7D47-A967-3BFA25C03DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7380" yWindow="-28300" windowWidth="40840" windowHeight="25880" xr2:uid="{773DC8B7-C252-694E-94F4-594B4B2CBB52}"/>
+    <workbookView xWindow="10920" yWindow="-26580" windowWidth="39540" windowHeight="25880" xr2:uid="{773DC8B7-C252-694E-94F4-594B4B2CBB52}"/>
   </bookViews>
   <sheets>
     <sheet name="Eastern" sheetId="1" r:id="rId1"/>
@@ -779,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{212F6219-047C-134A-8547-629CC30498DE}">
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="167" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>